<commit_message>
adding metadata information and classes
</commit_message>
<xml_diff>
--- a/src/test_data/services_1.xlsx
+++ b/src/test_data/services_1.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17220" tabRatio="500"/>
+    <workbookView xWindow="58620" yWindow="1340" windowWidth="25360" windowHeight="17220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -136,7 +137,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,6 +161,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -178,22 +186,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -526,7 +543,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -799,4 +816,49 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2"/>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>